<commit_message>
Major updates to the text model, to the data collection. I still need to clean up the code. Now it is all over the place
</commit_message>
<xml_diff>
--- a/DCF_Model.xlsx
+++ b/DCF_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maseehfaizan/Desktop/Maseeh/Projects/Hybrid_Pricer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C65511-C0EB-4E47-9D2E-ADBE2B9A7D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809E154B-E6CB-6749-BB02-58661439DC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="660" windowWidth="25380" windowHeight="26920" activeTab="1" xr2:uid="{5C6AE20B-A485-1C4F-988C-630508701A62}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="14160" windowHeight="16100" activeTab="1" xr2:uid="{5C6AE20B-A485-1C4F-988C-630508701A62}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -1298,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A77CE5-09E0-4342-81F4-D434F90C6B0A}">
   <dimension ref="A1:CF7"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AR1" sqref="AR1"/>
+    <sheetView topLeftCell="AN1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="BF1" sqref="BF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3092,7 +3092,7 @@
   <dimension ref="B1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3490,23 +3490,23 @@
         <v>102</v>
       </c>
       <c r="C16" cm="1">
-        <f t="array" ref="C16:H16">TRANSPOSE(test!BR2:BR7)</f>
-        <v>8400000000</v>
+        <f t="array" ref="C16:H16">TRANSPOSE(test!AW2:AW7)</f>
+        <v>4448000000</v>
       </c>
       <c r="D16">
-        <v>12500000000</v>
+        <v>8755000000</v>
       </c>
       <c r="E16">
-        <v>13400000000</v>
+        <v>9831000000</v>
       </c>
       <c r="F16">
-        <v>16000000000</v>
+        <v>10978000000</v>
       </c>
       <c r="G16">
-        <v>23100000000</v>
+        <v>16950000000</v>
       </c>
       <c r="H16">
-        <v>23400000000</v>
+        <v>19651000000</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
@@ -3760,20 +3760,20 @@
         <v>-829000000</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" ref="E27:H27" si="18">(E26-D26)/D26</f>
-        <v>0.19367514970059879</v>
+        <f t="shared" ref="E27:H27" si="18">(E26-D26)</f>
+        <v>4140000000</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="18"/>
-        <v>0.13665935099545384</v>
+        <v>3487000000</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="18"/>
-        <v>0.14101989449367308</v>
+        <v>4090000000</v>
       </c>
       <c r="H27" s="5">
         <f t="shared" si="18"/>
-        <v>9.3101260085214396E-2</v>
+        <v>3081000000</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
@@ -3834,24 +3834,24 @@
         <v>111</v>
       </c>
       <c r="D30">
-        <f t="shared" ref="D30:H30" si="20">D15-D16-D17+D18-D27-D28</f>
-        <v>38147000000</v>
+        <f t="shared" ref="D30:G30" si="20">D15-D16-D17+D18-D28-D27</f>
+        <v>41892000000</v>
       </c>
       <c r="E30">
         <f t="shared" si="20"/>
-        <v>46793999999.806328</v>
+        <v>46223000000</v>
       </c>
       <c r="F30">
         <f t="shared" si="20"/>
-        <v>58096999999.863342</v>
+        <v>59632000000</v>
       </c>
       <c r="G30">
         <f t="shared" si="20"/>
-        <v>50815999999.858978</v>
+        <v>52876000000</v>
       </c>
       <c r="H30">
-        <f t="shared" si="20"/>
-        <v>61555999999.906906</v>
+        <f>H15-H16-H17+H18-H28-H27</f>
+        <v>62224000000</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>